<commit_message>
Combinar con scripts database y bonds
</commit_message>
<xml_diff>
--- a/movimientos.xlsx
+++ b/movimientos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marqu\Documents\scripts\portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C10F91-F884-49CF-850E-82C9BA4EE736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E82EE57-E8AD-4460-82FC-7F0C4AB04B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{83537EAC-69F8-40CC-8901-C486DF30A447}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="44">
   <si>
     <t>compra</t>
   </si>
@@ -130,6 +130,42 @@
   </si>
   <si>
     <t>GGAL.BA</t>
+  </si>
+  <si>
+    <t>USD MEP</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>bono</t>
+  </si>
+  <si>
+    <t>AL35</t>
+  </si>
+  <si>
+    <t>fci</t>
+  </si>
+  <si>
+    <t>RJMULIA</t>
+  </si>
+  <si>
+    <t>TB21</t>
+  </si>
+  <si>
+    <t>TX21</t>
+  </si>
+  <si>
+    <t>TX22</t>
+  </si>
+  <si>
+    <t>GD41</t>
+  </si>
+  <si>
+    <t>AA22</t>
+  </si>
+  <si>
+    <t>TV22</t>
   </si>
 </sst>
 </file>
@@ -487,10 +523,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4F1DED-6426-4BD8-AF43-5C89B34FA00D}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,23 +592,23 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2">
-        <v>5</v>
-      </c>
-      <c r="G3" s="2">
-        <v>871.07</v>
+        <v>33</v>
+      </c>
+      <c r="F3" s="3">
+        <v>310.92</v>
+      </c>
+      <c r="G3">
+        <v>160.99247394828299</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H19" si="0">F3*G3</f>
-        <v>4355.3500000000004</v>
+        <f>F3*G3</f>
+        <v>50055.780000000152</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -585,25 +622,25 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G4" s="2">
-        <v>4113.67</v>
+        <v>871.07</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="0"/>
-        <v>16454.68</v>
+        <f>F4*G4</f>
+        <v>4355.3500000000004</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>44347</v>
+        <v>44337</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -612,47 +649,47 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G5" s="2">
-        <v>3818.12</v>
+        <v>4113.67</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="0"/>
-        <v>7636.24</v>
+        <f>F5*G5</f>
+        <v>16454.68</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>44347</v>
+        <v>44343</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2">
-        <v>2</v>
-      </c>
-      <c r="G6" s="2">
-        <v>3753.16</v>
+      <c r="F6" s="3">
+        <v>200</v>
+      </c>
+      <c r="G6">
+        <v>53.79</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>7506.32</v>
+        <f>F6*G6</f>
+        <v>10758</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -666,7 +703,7 @@
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -675,92 +712,91 @@
         <v>2</v>
       </c>
       <c r="G7" s="2">
-        <v>2091.58</v>
+        <v>3818.12</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="0"/>
-        <v>4183.16</v>
+        <f>F7*G7</f>
+        <v>7636.24</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>44362</v>
+        <v>44347</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2">
-        <v>12</v>
-      </c>
       <c r="G8" s="2">
-        <v>169.13</v>
+        <v>3753.16</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="0"/>
-        <v>2029.56</v>
+        <f>F8*G8</f>
+        <v>7506.32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>44362</v>
+        <v>44347</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="2">
-        <v>30</v>
-      </c>
       <c r="G9" s="2">
-        <v>74.52</v>
+        <v>2091.58</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="0"/>
-        <v>2235.6</v>
+        <f>F9*G9</f>
+        <v>4183.16</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>44362</v>
+        <v>44350</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>926.46</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="0"/>
-        <v>2779.38</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -774,160 +810,160 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="2">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="G11" s="2">
-        <v>49.34</v>
+        <v>169.13</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>1973.6000000000001</v>
+        <f>F11*G11</f>
+        <v>2029.56</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>44400</v>
+        <v>44362</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="2">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G12" s="2">
-        <v>5765.18</v>
+        <v>74.52</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="0"/>
-        <v>5765.18</v>
+        <f>F12*G12</f>
+        <v>2235.6</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>44400</v>
+        <v>44362</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G13" s="2">
-        <v>7894.02</v>
+        <v>926.46</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>7894.02</v>
+        <f>F13*G13</f>
+        <v>2779.38</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>44400</v>
+        <v>44362</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="2">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="G14" s="2">
-        <v>7889.99</v>
+        <v>49.34</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="0"/>
-        <v>7889.99</v>
+        <f>F14*G14</f>
+        <v>1973.6000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>44400</v>
+        <v>44398</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="2">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2">
-        <v>3532.62</v>
+      <c r="F15">
+        <v>2000</v>
+      </c>
+      <c r="G15">
+        <v>1.08</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="0"/>
-        <v>7065.24</v>
+        <f t="shared" ref="H15:H16" si="0">F15*G15</f>
+        <v>2160</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>44421</v>
+        <v>44398</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="2">
-        <v>16</v>
-      </c>
-      <c r="G16" s="2">
-        <v>62.44</v>
+      <c r="F16">
+        <v>1000</v>
+      </c>
+      <c r="G16">
+        <v>1.7</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="0"/>
-        <v>999.04</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>44421</v>
+        <v>44400</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -936,7 +972,7 @@
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -945,16 +981,16 @@
         <v>1</v>
       </c>
       <c r="G17" s="2">
-        <v>2003.96</v>
+        <v>5765.18</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="0"/>
-        <v>2003.96</v>
+        <f>F17*G17</f>
+        <v>5765.18</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>44426</v>
+        <v>44400</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -963,25 +999,25 @@
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="2">
-        <v>2735.07</v>
+        <v>7894.02</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="0"/>
-        <v>5470.14</v>
+        <f>F18*G18</f>
+        <v>7894.02</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44475</v>
+        <v>44400</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -990,7 +1026,7 @@
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
@@ -999,11 +1035,281 @@
         <v>1</v>
       </c>
       <c r="G19" s="2">
+        <v>7889.99</v>
+      </c>
+      <c r="H19" s="2">
+        <f>F19*G19</f>
+        <v>7889.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44400</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2</v>
+      </c>
+      <c r="G20" s="2">
+        <v>3532.62</v>
+      </c>
+      <c r="H20" s="2">
+        <f>F20*G20</f>
+        <v>7065.24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44420</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>2000</v>
+      </c>
+      <c r="G21">
+        <v>1.66</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" ref="H21" si="1">F21*G21</f>
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>44420</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>80</v>
+      </c>
+      <c r="G22">
+        <v>67.92</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" ref="H22" si="2">F22*G22</f>
+        <v>5433.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>44420</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>217</v>
+      </c>
+      <c r="G23">
+        <v>1.02</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" ref="H23" si="3">F23*G23</f>
+        <v>221.34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>44421</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="2">
+        <v>16</v>
+      </c>
+      <c r="G24" s="2">
+        <v>62.44</v>
+      </c>
+      <c r="H24" s="2">
+        <f>F24*G24</f>
+        <v>999.04</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>44421</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+      <c r="G25">
+        <v>98.04</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" ref="H25" si="4">F25*G25</f>
+        <v>1960.8000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>44421</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2">
+        <v>2003.96</v>
+      </c>
+      <c r="H26" s="2">
+        <f>F26*G26</f>
+        <v>2003.96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>44426</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="2">
+        <v>2</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2735.07</v>
+      </c>
+      <c r="H27" s="2">
+        <f>F27*G27</f>
+        <v>5470.14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>44475</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
         <v>7834.6</v>
       </c>
-      <c r="H19" s="2">
-        <f t="shared" si="0"/>
+      <c r="H28" s="2">
+        <f t="shared" ref="H28" si="5">F28*G28</f>
         <v>7834.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>44476</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="3">
+        <v>71.64</v>
+      </c>
+      <c r="G29">
+        <v>182.09226689000599</v>
+      </c>
+      <c r="H29" s="2">
+        <f>F29*G29</f>
+        <v>13045.090000000029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ya agregue bonos, mep y ccl, estoy viendo como agregar pagos por intereses y amortizaciones
</commit_message>
<xml_diff>
--- a/movimientos.xlsx
+++ b/movimientos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marqu\Documents\scripts\portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E82EE57-E8AD-4460-82FC-7F0C4AB04B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3557D78A-3A0C-42CF-90C5-043E5488E8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{83537EAC-69F8-40CC-8901-C486DF30A447}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>VIST</t>
   </si>
   <si>
-    <t>ALUA</t>
-  </si>
-  <si>
     <t>PBR</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>TV22</t>
+  </si>
+  <si>
+    <t>ALUA.BA</t>
   </si>
 </sst>
 </file>
@@ -526,8 +526,8 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,10 +595,10 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
       </c>
       <c r="F3" s="3">
         <v>310.92</v>
@@ -607,7 +607,7 @@
         <v>160.99247394828299</v>
       </c>
       <c r="H3" s="2">
-        <f>F3*G3</f>
+        <f t="shared" ref="H3:H9" si="0">F3*G3</f>
         <v>50055.780000000152</v>
       </c>
     </row>
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -634,7 +634,7 @@
         <v>871.07</v>
       </c>
       <c r="H4" s="2">
-        <f>F4*G4</f>
+        <f t="shared" si="0"/>
         <v>4355.3500000000004</v>
       </c>
     </row>
@@ -646,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -661,7 +661,7 @@
         <v>4113.67</v>
       </c>
       <c r="H5" s="2">
-        <f>F5*G5</f>
+        <f t="shared" si="0"/>
         <v>16454.68</v>
       </c>
     </row>
@@ -673,10 +673,10 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
         <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -688,7 +688,7 @@
         <v>53.79</v>
       </c>
       <c r="H6" s="2">
-        <f>F6*G6</f>
+        <f t="shared" si="0"/>
         <v>10758</v>
       </c>
     </row>
@@ -700,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -715,7 +715,7 @@
         <v>3818.12</v>
       </c>
       <c r="H7" s="2">
-        <f>F7*G7</f>
+        <f t="shared" si="0"/>
         <v>7636.24</v>
       </c>
     </row>
@@ -727,7 +727,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -742,7 +742,7 @@
         <v>3753.16</v>
       </c>
       <c r="H8" s="2">
-        <f>F8*G8</f>
+        <f t="shared" si="0"/>
         <v>7506.32</v>
       </c>
     </row>
@@ -754,7 +754,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -769,7 +769,7 @@
         <v>2091.58</v>
       </c>
       <c r="H9" s="2">
-        <f>F9*G9</f>
+        <f t="shared" si="0"/>
         <v>4183.16</v>
       </c>
     </row>
@@ -781,10 +781,10 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
         <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -810,7 +810,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -837,7 +837,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -864,7 +864,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -891,7 +891,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -915,10 +915,10 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -930,7 +930,7 @@
         <v>1.08</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" ref="H15:H16" si="0">F15*G15</f>
+        <f t="shared" ref="H15:H16" si="1">F15*G15</f>
         <v>2160</v>
       </c>
     </row>
@@ -942,10 +942,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
@@ -957,7 +957,7 @@
         <v>1.7</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1700</v>
       </c>
     </row>
@@ -969,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -996,7 +996,7 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1023,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1050,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1077,10 +1077,10 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
         <v>7</v>
@@ -1092,7 +1092,7 @@
         <v>1.66</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" ref="H21" si="1">F21*G21</f>
+        <f t="shared" ref="H21" si="2">F21*G21</f>
         <v>3320</v>
       </c>
     </row>
@@ -1104,10 +1104,10 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
@@ -1119,7 +1119,7 @@
         <v>67.92</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" ref="H22" si="2">F22*G22</f>
+        <f t="shared" ref="H22" si="3">F22*G22</f>
         <v>5433.6</v>
       </c>
     </row>
@@ -1131,10 +1131,10 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
@@ -1146,7 +1146,7 @@
         <v>1.02</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" ref="H23" si="3">F23*G23</f>
+        <f t="shared" ref="H23" si="4">F23*G23</f>
         <v>221.34</v>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
@@ -1185,10 +1185,10 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E25" t="s">
         <v>7</v>
@@ -1200,7 +1200,7 @@
         <v>98.04</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" ref="H25" si="4">F25*G25</f>
+        <f t="shared" ref="H25" si="5">F25*G25</f>
         <v>1960.8000000000002</v>
       </c>
     </row>
@@ -1212,10 +1212,10 @@
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
@@ -1239,10 +1239,10 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E27" t="s">
         <v>7</v>
@@ -1266,10 +1266,10 @@
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E28" t="s">
         <v>7</v>
@@ -1281,7 +1281,7 @@
         <v>7834.6</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" ref="H28" si="5">F28*G28</f>
+        <f t="shared" ref="H28" si="6">F28*G28</f>
         <v>7834.6</v>
       </c>
     </row>
@@ -1296,10 +1296,10 @@
         <v>14</v>
       </c>
       <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" t="s">
         <v>32</v>
-      </c>
-      <c r="E29" t="s">
-        <v>33</v>
       </c>
       <c r="F29" s="3">
         <v>71.64</v>

</xml_diff>